<commit_message>
This commit includes code for resolving data between a spreadsheet and the repository. Also added some exception handling.
Also fixed some swagger problems after the Spring Boot upgrade.
</commit_message>
<xml_diff>
--- a/src/test/resources/users.xlsx
+++ b/src/test/resources/users.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">Nona</t>
   </si>
   <si>
-    <t xml:space="preserve">ON</t>
+    <t xml:space="preserve">Alberta</t>
   </si>
   <si>
     <t xml:space="preserve">Emma</t>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Caitlin</t>
   </si>
   <si>
-    <t xml:space="preserve">BC</t>
+    <t xml:space="preserve">Colombie-Britannique</t>
   </si>
 </sst>
 </file>
@@ -61,6 +61,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -125,7 +126,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -149,30 +150,33 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.68"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -180,10 +184,10 @@
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>